<commit_message>
modified pom pages modified pom pages#
</commit_message>
<xml_diff>
--- a/CarWale/Inputdata/SUV_Details.xlsx
+++ b/CarWale/Inputdata/SUV_Details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sunit\eclipse-workspace\CarWale\Inputdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B99E1F-B2D0-42E4-A011-3E889CE5A396}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34171428-711A-4FDA-B3F8-73752CF1EA4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5070" yWindow="2070" windowWidth="15375" windowHeight="8850" xr2:uid="{46DF8180-ABFA-4B68-AD48-8E347EBF173D}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>VersionsOfVehicle</t>
   </si>
@@ -53,6 +53,15 @@
     <t>₹ 6.31 Lakh</t>
   </si>
   <si>
+    <t>Renault Kiger</t>
+  </si>
+  <si>
+    <t>Kiger RXE MT</t>
+  </si>
+  <si>
+    <t>₹ 5.45 Lakh</t>
+  </si>
+  <si>
     <t>Venue S 1.2 Petrol</t>
   </si>
   <si>
@@ -69,6 +78,15 @@
   </si>
   <si>
     <t>₹ 8.46 Lakh</t>
+  </si>
+  <si>
+    <t>Hyundai Venue</t>
+  </si>
+  <si>
+    <t>Hyundai Venue E 1.2 Petrol</t>
+  </si>
+  <si>
+    <t>₹ 6.87 Lakh</t>
   </si>
 </sst>
 </file>
@@ -437,7 +455,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -479,6 +497,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -486,13 +520,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.4765625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.62890625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="14.9921875" collapsed="true"/>
   </cols>
   <sheetData>
@@ -506,26 +540,42 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>